<commit_message>
all type of scheme done
</commit_message>
<xml_diff>
--- a/public/discussion/POS_Table_Structure.xlsx
+++ b/public/discussion/POS_Table_Structure.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="113">
   <si>
     <t>Column Name</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>Amt (Rs. 2/-)</t>
-  </si>
-  <si>
-    <t>Perc (3%)</t>
   </si>
   <si>
     <t>Item_code</t>
@@ -453,6 +450,15 @@
   </si>
   <si>
     <t>Narendra (Amt/%) - Rs. 0</t>
+  </si>
+  <si>
+    <t>Perc (5%)</t>
+  </si>
+  <si>
+    <t>Value3</t>
+  </si>
+  <si>
+    <t>Fix (Rs 23/-)</t>
   </si>
 </sst>
 </file>
@@ -833,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -934,30 +940,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -992,12 +974,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1005,6 +981,42 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1317,7 +1329,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1325,11 +1337,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,15 +1352,15 @@
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1370,8 +1382,11 @@
       <c r="G1" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
@@ -1389,8 +1404,11 @@
       <c r="G2" s="12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H2" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>22</v>
       </c>
@@ -1408,8 +1426,11 @@
       <c r="G3" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
@@ -1427,8 +1448,11 @@
       <c r="G4" s="16">
         <v>44573</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H4" s="16">
+        <v>44573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -1446,8 +1470,11 @@
       <c r="G5" s="14" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H5" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>34</v>
       </c>
@@ -1469,8 +1496,11 @@
       <c r="G6" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H6" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>26</v>
       </c>
@@ -1488,8 +1518,11 @@
       <c r="G7" s="14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H7" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
@@ -1507,8 +1540,11 @@
       <c r="G8" s="14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H8" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>37</v>
       </c>
@@ -1526,8 +1562,11 @@
       <c r="G9" s="14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H9" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>29</v>
       </c>
@@ -1549,15 +1588,18 @@
       <c r="G10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" t="s">
+      <c r="H10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" t="s">
         <v>98</v>
       </c>
-      <c r="L10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -1571,25 +1613,29 @@
       <c r="E11" s="10"/>
       <c r="F11" s="18">
         <f>SUM(F39:G39)</f>
-        <v>6.1999999999999993</v>
+        <v>51.325000000000003</v>
       </c>
       <c r="G11" s="19">
         <f>SUM(F39:G39)</f>
-        <v>6.1999999999999993</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="J11" s="6">
+        <v>51.325000000000003</v>
+      </c>
+      <c r="H11" s="19">
+        <f>SUM(G39:H39)</f>
+        <v>45.125</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="6">
         <v>1</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6">
+      <c r="L11" s="6"/>
+      <c r="M11" s="6">
         <v>5</v>
       </c>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -1603,25 +1649,29 @@
       <c r="E12" s="10"/>
       <c r="F12" s="18">
         <f>ROUND(F11,0)-F11</f>
-        <v>-0.19999999999999929</v>
+        <v>-0.32500000000000284</v>
       </c>
       <c r="G12" s="19">
         <f>ROUND(G11,0)-G11</f>
-        <v>-0.19999999999999929</v>
-      </c>
-      <c r="I12" s="6" t="s">
+        <v>-0.32500000000000284</v>
+      </c>
+      <c r="H12" s="19">
+        <f>ROUND(H11,0)-H11</f>
+        <v>-0.125</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="6">
+      <c r="K12" s="6">
         <v>2</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6">
+      <c r="L12" s="6"/>
+      <c r="M12" s="6">
         <v>4</v>
       </c>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>30</v>
       </c>
@@ -1635,25 +1685,29 @@
       <c r="E13" s="10"/>
       <c r="F13" s="18">
         <f>F11+F12</f>
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="G13" s="20">
         <f>G11+G12</f>
-        <v>6</v>
-      </c>
-      <c r="I13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="20">
+        <f>H11+H12</f>
+        <v>45</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="6">
+      <c r="K13" s="6">
         <v>50</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6">
+      <c r="L13" s="6"/>
+      <c r="M13" s="6">
         <v>25</v>
       </c>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>31</v>
       </c>
@@ -1671,19 +1725,22 @@
       <c r="G14" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J14" s="6">
+      <c r="K14" s="6">
         <v>32</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6">
+      <c r="L14" s="6"/>
+      <c r="M14" s="6">
         <v>16</v>
       </c>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
@@ -1701,19 +1758,22 @@
       <c r="G15" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K15" s="6">
         <v>45</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6">
+      <c r="L15" s="6"/>
+      <c r="M15" s="6">
         <v>22</v>
       </c>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>33</v>
       </c>
@@ -1731,21 +1791,24 @@
       <c r="G16" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="H16" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J16" s="6">
-        <f>J15*J12</f>
+      <c r="K16" s="6">
+        <f>K15*K12</f>
         <v>90</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6">
-        <f>L15*L12</f>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6">
+        <f>M15*M12</f>
         <v>88</v>
       </c>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>35</v>
       </c>
@@ -1763,10 +1826,13 @@
       <c r="G17" s="14">
         <v>1</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H17" s="14">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>36</v>
       </c>
@@ -1784,25 +1850,28 @@
       <c r="G18" s="14">
         <v>1</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="J18" s="6">
-        <f>2*J12</f>
+      <c r="H18" s="14">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" s="6">
+        <f>2*K12</f>
         <v>4</v>
       </c>
-      <c r="K18" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="L18" s="6">
-        <f>(L16*3)/100</f>
+      <c r="L18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M18" s="6">
+        <f>(M16*3)/100</f>
         <v>2.64</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N18" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>38</v>
       </c>
@@ -1824,21 +1893,24 @@
       <c r="G19" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" s="6">
-        <f>J16-J18</f>
+      <c r="H19" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19" s="6">
+        <f>K16-K18</f>
         <v>86</v>
       </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6">
-        <f>L16-L18</f>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6">
+        <f>M16-M18</f>
         <v>85.36</v>
       </c>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>43</v>
       </c>
@@ -1856,10 +1928,13 @@
       <c r="G20" s="28">
         <v>5</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H20" s="28">
+        <v>5</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>44</v>
       </c>
@@ -1877,25 +1952,28 @@
       <c r="G21" s="30">
         <v>87648754</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J21" s="6">
-        <f>(J16*5)/100</f>
+      <c r="H21" s="30">
+        <v>87648754</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="6">
+        <f>(K16*5)/100</f>
         <v>4.5</v>
       </c>
-      <c r="K21" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="L21" s="6">
-        <f>(L16*0)/100</f>
+      <c r="L21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M21" s="6">
+        <f>(M16*0)/100</f>
         <v>0</v>
       </c>
-      <c r="M21" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N21" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>45</v>
       </c>
@@ -1911,23 +1989,26 @@
         <v>1</v>
       </c>
       <c r="G22" s="30">
-        <v>0</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="J22" s="6">
-        <f>J19-J21</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="30">
+        <v>1</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K22" s="6">
+        <f>K19-K21</f>
         <v>81.5</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6">
-        <f>L19-L21</f>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6">
+        <f>M19-M21</f>
         <v>85.36</v>
       </c>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>48</v>
       </c>
@@ -1943,12 +2024,15 @@
         <v>10</v>
       </c>
       <c r="G23" s="30">
+        <v>50</v>
+      </c>
+      <c r="H23" s="30">
         <v>25</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23"/>
-    </row>
-    <row r="24" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J23" s="3"/>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>53</v>
       </c>
@@ -1964,22 +2048,25 @@
         <v>7.2</v>
       </c>
       <c r="G24" s="30">
-        <v>16</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J24" s="48">
-        <f>J22+L22</f>
+        <v>35.19</v>
+      </c>
+      <c r="H24" s="30">
+        <v>17.5</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="75">
+        <f>K22+M22</f>
         <v>166.86</v>
       </c>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="50"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-    </row>
-    <row r="25" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="L24" s="76"/>
+      <c r="M24" s="76"/>
+      <c r="N24" s="77"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="68"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>54</v>
       </c>
@@ -1995,12 +2082,15 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G25" s="30">
-        <v>22</v>
-      </c>
-      <c r="I25" s="3"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+      <c r="H25" s="30">
+        <v>23.8</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>46</v>
       </c>
@@ -2018,20 +2108,24 @@
       </c>
       <c r="G26" s="30">
         <f>G22*G25</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J26" s="48">
-        <f>(J24*5)/100</f>
+        <v>47.5</v>
+      </c>
+      <c r="H26" s="30">
+        <f>H22*H25</f>
+        <v>23.8</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K26" s="75">
+        <f>(K24*5)/100</f>
         <v>8.343</v>
       </c>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="50"/>
-    </row>
-    <row r="27" spans="1:17" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="77"/>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>47</v>
       </c>
@@ -2049,205 +2143,225 @@
       <c r="G27" s="33">
         <v>345</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="J27" s="7">
-        <f>(J22*5)/100</f>
+      <c r="H27" s="33">
+        <v>345</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K27" s="7">
+        <f>(K22*5)/100</f>
         <v>4.0750000000000002</v>
       </c>
-      <c r="K27" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="L27" s="7">
-        <f>(L22*5)/100</f>
+      <c r="L27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M27" s="7">
+        <f>(M22*5)/100</f>
         <v>4.2679999999999998</v>
       </c>
-      <c r="M27" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A28" s="62" t="s">
+      <c r="N27" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="63">
+      <c r="B28" s="55">
         <v>27</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="63" t="s">
+      <c r="D28" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="63" t="s">
+      <c r="E28" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="64" t="s">
+      <c r="F28" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="G28" s="65" t="s">
-        <v>84</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J28" s="7">
-        <f>J22-J27</f>
+      <c r="G28" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="H28" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K28" s="7">
+        <f>K22-K27</f>
         <v>77.424999999999997</v>
       </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="7">
-        <f>L22-L27</f>
+      <c r="L28" s="6"/>
+      <c r="M28" s="7">
+        <f>M22-M27</f>
         <v>81.091999999999999</v>
       </c>
-      <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="1:17" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="66" t="s">
+      <c r="N28" s="6"/>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="67">
+      <c r="B29" s="59">
         <v>28</v>
       </c>
-      <c r="C29" s="67" t="s">
+      <c r="C29" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" s="68">
+      <c r="D29" s="59"/>
+      <c r="E29" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="60">
         <f>2*F22</f>
         <v>2</v>
       </c>
-      <c r="G29" s="69">
-        <f>(G26*3)/100</f>
+      <c r="G29" s="61">
+        <f>(G26*5)/100</f>
+        <v>2.375</v>
+      </c>
+      <c r="H29" s="61">
+        <f>H25-H3023</f>
+        <v>23.8</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="47">
+        <v>29</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="47"/>
+      <c r="E30" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="46">
         <v>0</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A30" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="55">
-        <v>29</v>
-      </c>
-      <c r="C30" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="54">
-        <v>0</v>
-      </c>
-      <c r="G30" s="57"/>
-      <c r="I30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="J30" s="48">
-        <f>J28+L28</f>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="J30" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K30" s="75">
+        <f>K28+M28</f>
         <v>158.517</v>
       </c>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="50"/>
-    </row>
-    <row r="31" spans="1:17" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="58" t="s">
+      <c r="L30" s="76"/>
+      <c r="M30" s="76"/>
+      <c r="N30" s="77"/>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="59">
+      <c r="B31" s="51">
         <v>30</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" s="60">
+      <c r="D31" s="51"/>
+      <c r="E31" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="52">
         <f>(F26*F30)/100</f>
         <v>0</v>
       </c>
-      <c r="G31" s="61">
+      <c r="G31" s="53">
         <f>(G26*G30)/100</f>
         <v>0</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A32" s="70" t="s">
+      <c r="H31" s="53">
+        <f>(H26*H30)/100</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="71">
+      <c r="B32" s="63">
         <v>31</v>
       </c>
-      <c r="C32" s="71" t="s">
+      <c r="C32" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" s="73"/>
-      <c r="I32" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J32" s="8">
-        <f>(6/J30)*100</f>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="G32" s="70"/>
+      <c r="H32" s="78"/>
+      <c r="J32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K32" s="8">
+        <f>(6/K30)*100</f>
         <v>3.7850829879445111</v>
       </c>
-      <c r="K32" s="8"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="74" t="s">
+      <c r="M32" s="8"/>
+      <c r="N32" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="75">
+      <c r="B33" s="65">
         <v>32</v>
       </c>
-      <c r="C33" s="75" t="s">
+      <c r="C33" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75" t="s">
+      <c r="D33" s="65"/>
+      <c r="E33" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="76">
+      <c r="F33" s="66">
         <f>((F26-F29-F31)*0)/100</f>
         <v>0</v>
       </c>
-      <c r="G33" s="77">
+      <c r="G33" s="67">
         <f>((G26-G29-G31)*0)/100</f>
         <v>0</v>
       </c>
-      <c r="I33" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J33" s="7">
-        <f>(J28*J32)/100</f>
+      <c r="H33" s="67">
+        <f>((H26-H29-H31)*0)/100</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K33" s="7">
+        <f>(K28*K32)/100</f>
         <v>2.9306005034160374</v>
       </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="7">
-        <f>(L28*J32)/100</f>
+      <c r="L33" s="6"/>
+      <c r="M33" s="7">
+        <f>(M28*K32)/100</f>
         <v>3.069399496583963</v>
       </c>
-      <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
         <v>52</v>
       </c>
@@ -2265,10 +2379,13 @@
       <c r="G34" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34"/>
-    </row>
-    <row r="35" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H34" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="s">
         <v>78</v>
       </c>
@@ -2280,25 +2397,26 @@
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="35"/>
-      <c r="F35" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="G35" s="53"/>
-      <c r="I35" s="6" t="s">
+      <c r="F35" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" s="72"/>
+      <c r="H35" s="79"/>
+      <c r="J35" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="J35" s="7">
-        <f>J28+J33</f>
+      <c r="K35" s="7">
+        <f>K28+K33</f>
         <v>80.355600503416028</v>
       </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="7">
-        <f>L28+L33</f>
+      <c r="L35" s="6"/>
+      <c r="M35" s="7">
+        <f>M28+M33</f>
         <v>84.161399496583968</v>
       </c>
-      <c r="M35" s="6"/>
-    </row>
-    <row r="36" spans="1:13" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
         <v>79</v>
       </c>
@@ -2320,21 +2438,25 @@
         <f>(G26-G29-G31)*(0/((F26-F29-F31)+(G26-G29-G31))*100)/100</f>
         <v>0</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="H36" s="45">
+        <f>(H26-H29-H31)*(0/((G26-G29-G31)+(H26-H29-H31))*100)/100</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="J36" s="7">
-        <f>J35/J12</f>
+      <c r="K36" s="7">
+        <f>K35/K12</f>
         <v>40.177800251708014</v>
       </c>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7">
-        <f>L35/L12</f>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7">
+        <f>M35/M12</f>
         <v>21.040349874145992</v>
       </c>
-      <c r="M36" s="6"/>
-    </row>
-    <row r="37" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="N36" s="6"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>50</v>
       </c>
@@ -2352,10 +2474,13 @@
       <c r="G37" s="42">
         <v>0.12</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37"/>
-    </row>
-    <row r="38" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H37" s="42">
+        <v>0.12</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>51</v>
       </c>
@@ -2373,18 +2498,21 @@
       <c r="G38" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I38" s="6" t="s">
+      <c r="H38" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="J38" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J38" s="46">
-        <f>J35+L35</f>
+      <c r="K38" s="73">
+        <f>K35+M35</f>
         <v>164.517</v>
       </c>
-      <c r="K38" s="47"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="47"/>
-    </row>
-    <row r="39" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="L38" s="74"/>
+      <c r="M38" s="74"/>
+      <c r="N38" s="74"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>72</v>
       </c>
@@ -2402,21 +2530,25 @@
       </c>
       <c r="G39" s="44">
         <f>(G26-G29-G31-G33+G36)</f>
+        <v>45.125</v>
+      </c>
+      <c r="H39" s="44">
+        <f>(H26-H29-H31-H33+H36)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="J39" s="46">
-        <f>ROUND(J38,0)-J38</f>
+      <c r="I39" s="5"/>
+      <c r="J39" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K39" s="73">
+        <f>ROUND(K38,0)-K38</f>
         <v>0.48300000000000409</v>
       </c>
-      <c r="K39" s="47"/>
-      <c r="L39" s="47"/>
-      <c r="M39" s="47"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L39" s="74"/>
+      <c r="M39" s="74"/>
+      <c r="N39" s="74"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>70</v>
       </c>
@@ -2432,22 +2564,26 @@
         <f>F39/F22</f>
         <v>6.1999999999999993</v>
       </c>
-      <c r="G40" s="44" t="e">
+      <c r="G40" s="44">
         <f>G39/G22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I40" s="6" t="s">
+        <v>45.125</v>
+      </c>
+      <c r="H40" s="44">
+        <f>H39/H22</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J40" s="46">
-        <f>J38+J39</f>
+      <c r="K40" s="73">
+        <f>K38+K39</f>
         <v>165</v>
       </c>
-      <c r="K40" s="47"/>
-      <c r="L40" s="47"/>
-      <c r="M40" s="47"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L40" s="74"/>
+      <c r="M40" s="74"/>
+      <c r="N40" s="74"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>28</v>
       </c>
@@ -2465,10 +2601,13 @@
       <c r="G41" s="30" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42" s="37">
         <v>41</v>
@@ -2484,18 +2623,21 @@
       <c r="G42" s="39" t="s">
         <v>73</v>
       </c>
+      <c r="H42" s="39" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="Q24:R24"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="F35:G35"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K38:N38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2620,7 +2762,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8">
         <v>7</v>

</xml_diff>